<commit_message>
modify card holder NIS
</commit_message>
<xml_diff>
--- a/images/noon/CardHolder/production/NIS.xlsx
+++ b/images/noon/CardHolder/production/NIS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sage\PycharmProjects\noon-images\images\noon\CardHolder\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27EE037-7E8E-46E9-8CC6-24361328C657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2C0EEF-E0AF-42FE-947C-38476D36D46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1013,7 +1013,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="947">
   <si>
     <t>How do I fill in the template tab?</t>
   </si>
@@ -3759,12 +3759,165 @@
   <si>
     <t>Generic</t>
   </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Almond%20Blossoms%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Almond%20Blossoms%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Almond%20Blossoms%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Almond%20Blossoms%20-%204.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20A%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20A%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20A%20-%204.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20B%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20B%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20B%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20B%20-%204.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20over%20the%20Rhone%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20over%20the%20Rhone%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Starry%20Night%20over%20the%20Rhone%20-%204.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Sunflowers%20A%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Sunflowers%20A%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Sunflowers%20A%20-%204.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Sunflowers%20B%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Sunflowers%20B%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Sunflowers%20B%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Van%20Gogh/Card%20Holder%20with%20Lanyard%20-%20Van%20Gogh%20-%20Sunflowers%20B%20-%204.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20Rabbit%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20Rabbit%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20Rabbit%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20Snorlax%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20Snorlax%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20Snorlax%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20the%20Mysterious%20Girl%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20the%20Mysterious%20Girl%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20and%20the%20Mysterious%20Girl%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20on%20Grassland%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20on%20Grassland%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Lanyard%20-%20Totoro%20on%20Grassland%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20Rabbit%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20Rabbit%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20Rabbit%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20Snorlax%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20Snorlax%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20Snorlax%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20the%20Mysterious%20Girl%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20the%20Mysterious%20Girl%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20and%20the%20Mysterious%20Girl%20-%203.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20on%20Grassland%20-%201.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20on%20Grassland%20-%202.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/CardHolder/production/Totoro/Card%20Holder%20with%20Wrist%20Strap%20-%20Totoro%20on%20Grassland%20-%203.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3831,6 +3984,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -4075,7 +4236,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
@@ -4084,8 +4245,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4148,18 +4310,61 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4171,54 +4376,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="8"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="GRAY_BACK_GROUND" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="GREEN_BACK_GROUND" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="LIGHT_GRAY_BACK_GROUND" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -4227,57 +4390,9 @@
     <cellStyle name="RED_BACK_GROUND" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="YELLOW_BACK_GROUND" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="8" builtinId="8"/>
   </cellStyles>
-  <dxfs count="306">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFA9A9A9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFDFDF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFF38D8D"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFF38D8D"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFF38D8D"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFFF0000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFDFFFDF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF006400"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF006400"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF006400"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF006400"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="303">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -9579,21 +9694,21 @@
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:29" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="28"/>
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
@@ -9674,21 +9789,21 @@
       <c r="AC3" s="12"/>
     </row>
     <row r="4" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
@@ -9707,21 +9822,21 @@
       <c r="AC4" s="14"/>
     </row>
     <row r="5" spans="1:29" ht="165" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28"/>
+      <c r="A5" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="32"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
       <c r="P5" s="15"/>
@@ -9740,19 +9855,19 @@
       <c r="AC5" s="15"/>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
@@ -9771,21 +9886,21 @@
       <c r="AC6" s="12"/>
     </row>
     <row r="7" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="32"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
@@ -9807,20 +9922,20 @@
       <c r="A8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="28"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="32"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
@@ -9842,20 +9957,20 @@
       <c r="A9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="28"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="32"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
@@ -9877,20 +9992,20 @@
       <c r="A10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="28"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
@@ -9909,19 +10024,19 @@
       <c r="AC10" s="17"/>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="32"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
@@ -9940,21 +10055,21 @@
       <c r="AC11" s="12"/>
     </row>
     <row r="12" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="32"/>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
@@ -9973,21 +10088,21 @@
       <c r="AC12" s="14"/>
     </row>
     <row r="13" spans="1:29" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="44"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
@@ -10006,19 +10121,19 @@
       <c r="AC13" s="15"/>
     </row>
     <row r="14" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="32"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
@@ -10037,21 +10152,21 @@
       <c r="AC14" s="12"/>
     </row>
     <row r="15" spans="1:29" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="41"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
@@ -10070,21 +10185,21 @@
       <c r="AC15" s="12"/>
     </row>
     <row r="16" spans="1:29" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
@@ -10144,20 +10259,20 @@
     </row>
     <row r="19" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20"/>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="32"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
       <c r="P19" s="14"/>
@@ -10177,20 +10292,20 @@
     </row>
     <row r="20" spans="1:29" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="32"/>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
@@ -10241,20 +10356,20 @@
     </row>
     <row r="22" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20"/>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="28"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32"/>
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
@@ -10274,20 +10389,20 @@
     </row>
     <row r="23" spans="1:29" ht="142.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="28"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
@@ -10338,20 +10453,20 @@
     </row>
     <row r="25" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="28"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="32"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
       <c r="P25" s="14"/>
@@ -10371,20 +10486,20 @@
     </row>
     <row r="26" spans="1:29" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="28"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="32"/>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
@@ -10466,20 +10581,20 @@
     </row>
     <row r="29" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="28"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="32"/>
       <c r="N29" s="14"/>
       <c r="O29" s="14"/>
       <c r="P29" s="14"/>
@@ -10499,20 +10614,20 @@
     </row>
     <row r="30" spans="1:29" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="28"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32"/>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
@@ -10532,18 +10647,18 @@
     </row>
     <row r="31" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="41"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="35"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
@@ -10563,20 +10678,20 @@
     </row>
     <row r="32" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="37"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="44"/>
       <c r="N32" s="14"/>
       <c r="O32" s="14"/>
       <c r="P32" s="14"/>
@@ -10596,20 +10711,20 @@
     </row>
     <row r="33" spans="1:29" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="28"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="32"/>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
@@ -10629,18 +10744,18 @@
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="41"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="35"/>
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
@@ -10659,21 +10774,21 @@
       <c r="AC34" s="12"/>
     </row>
     <row r="35" spans="1:29" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="28"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="32"/>
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -10692,21 +10807,21 @@
       <c r="AC35" s="10"/>
     </row>
     <row r="36" spans="1:29" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="28"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="32"/>
       <c r="N36" s="12"/>
       <c r="O36" s="12"/>
       <c r="P36" s="12"/>
@@ -10756,21 +10871,21 @@
       <c r="AC37" s="12"/>
     </row>
     <row r="38" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="28"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="32"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
@@ -10789,36 +10904,36 @@
       <c r="AC38" s="10"/>
     </row>
     <row r="39" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="47"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="41"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="35"/>
     </row>
     <row r="40" spans="1:29" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="28"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="32"/>
       <c r="N40" s="23"/>
       <c r="O40" s="23"/>
       <c r="P40" s="23"/>
@@ -10837,36 +10952,36 @@
       <c r="AC40" s="23"/>
     </row>
     <row r="41" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="47"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="41"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="35"/>
     </row>
     <row r="42" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="20"/>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="28"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="32"/>
       <c r="N42" s="14"/>
       <c r="O42" s="14"/>
       <c r="P42" s="14"/>
@@ -10886,20 +11001,20 @@
     </row>
     <row r="43" spans="1:29" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="28"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="32"/>
       <c r="N43" s="23"/>
       <c r="O43" s="23"/>
       <c r="P43" s="23"/>
@@ -10919,20 +11034,20 @@
     </row>
     <row r="44" spans="1:29" ht="127.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="28"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="32"/>
       <c r="N44" s="24"/>
       <c r="O44" s="24"/>
       <c r="P44" s="24"/>
@@ -10951,36 +11066,36 @@
       <c r="AC44" s="24"/>
     </row>
     <row r="45" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="41"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="35"/>
     </row>
     <row r="46" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="20"/>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="28"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="32"/>
       <c r="N46" s="14"/>
       <c r="O46" s="14"/>
       <c r="P46" s="14"/>
@@ -11000,20 +11115,20 @@
     </row>
     <row r="47" spans="1:29" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="25"/>
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="50"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="29"/>
       <c r="N47" s="23"/>
       <c r="O47" s="23"/>
       <c r="P47" s="23"/>
@@ -11034,6 +11149,36 @@
     <row r="48" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A7:M7"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="A12:M12"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="B22:M22"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="B25:M25"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="A35:M35"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="A45:M45"/>
+    <mergeCell ref="B46:M46"/>
     <mergeCell ref="B47:M47"/>
     <mergeCell ref="A38:M38"/>
     <mergeCell ref="A39:M39"/>
@@ -11042,36 +11187,6 @@
     <mergeCell ref="B42:M42"/>
     <mergeCell ref="B43:M43"/>
     <mergeCell ref="B44:M44"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="A35:M35"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="A45:M45"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="B32:M32"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="B22:M22"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B25:M25"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A15:M15"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="B19:M19"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:M10"/>
-    <mergeCell ref="A11:M11"/>
-    <mergeCell ref="A12:M12"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A7:M7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -11150,7 +11265,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -11632,7 +11747,7 @@
   <dimension ref="A1:CW25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11721,20 +11836,20 @@
       <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -11746,39 +11861,39 @@
       <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
     </row>
     <row r="4" spans="1:101" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
     </row>
     <row r="5" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -11790,20 +11905,20 @@
       <c r="D5" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
     </row>
     <row r="6" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
@@ -12891,7 +13006,7 @@
       <c r="C10" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="26" t="s">
         <v>879</v>
       </c>
       <c r="G10" t="s">
@@ -12920,6 +13035,18 @@
       </c>
       <c r="X10" t="s">
         <v>507</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>896</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>897</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>898</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>899</v>
       </c>
     </row>
     <row r="11" spans="1:101" x14ac:dyDescent="0.3">
@@ -12932,7 +13059,7 @@
       <c r="C11" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="26" t="s">
         <v>880</v>
       </c>
       <c r="G11" t="s">
@@ -12961,6 +13088,15 @@
       </c>
       <c r="X11" t="s">
         <v>507</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>900</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>901</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>902</v>
       </c>
     </row>
     <row r="12" spans="1:101" x14ac:dyDescent="0.3">
@@ -12973,7 +13109,7 @@
       <c r="C12" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="26" t="s">
         <v>881</v>
       </c>
       <c r="G12" t="s">
@@ -13002,6 +13138,18 @@
       </c>
       <c r="X12" t="s">
         <v>507</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>903</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>904</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>905</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>906</v>
       </c>
     </row>
     <row r="13" spans="1:101" x14ac:dyDescent="0.3">
@@ -13014,7 +13162,7 @@
       <c r="C13" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="26" t="s">
         <v>882</v>
       </c>
       <c r="G13" t="s">
@@ -13043,6 +13191,15 @@
       </c>
       <c r="X13" t="s">
         <v>507</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>907</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>908</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>909</v>
       </c>
     </row>
     <row r="14" spans="1:101" x14ac:dyDescent="0.3">
@@ -13055,7 +13212,7 @@
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="56" t="s">
+      <c r="E14" s="26" t="s">
         <v>883</v>
       </c>
       <c r="G14" t="s">
@@ -13084,6 +13241,15 @@
       </c>
       <c r="X14" t="s">
         <v>507</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>910</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>911</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>912</v>
       </c>
     </row>
     <row r="15" spans="1:101" x14ac:dyDescent="0.3">
@@ -13096,7 +13262,7 @@
       <c r="C15" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="26" t="s">
         <v>884</v>
       </c>
       <c r="G15" t="s">
@@ -13125,6 +13291,18 @@
       </c>
       <c r="X15" t="s">
         <v>507</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>913</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>914</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>915</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>916</v>
       </c>
     </row>
     <row r="16" spans="1:101" x14ac:dyDescent="0.3">
@@ -13137,7 +13315,7 @@
       <c r="C16" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="26" t="s">
         <v>885</v>
       </c>
       <c r="G16" t="s">
@@ -13167,8 +13345,17 @@
       <c r="X16" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF16" t="s">
+        <v>917</v>
+      </c>
+      <c r="AG16" s="57" t="s">
+        <v>918</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -13178,7 +13365,7 @@
       <c r="C17" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="26" t="s">
         <v>886</v>
       </c>
       <c r="G17" t="s">
@@ -13208,8 +13395,17 @@
       <c r="X17" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF17" t="s">
+        <v>920</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>921</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -13219,7 +13415,7 @@
       <c r="C18" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="26" t="s">
         <v>887</v>
       </c>
       <c r="G18" t="s">
@@ -13249,8 +13445,17 @@
       <c r="X18" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF18" t="s">
+        <v>923</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>924</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -13260,7 +13465,7 @@
       <c r="C19" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="26" t="s">
         <v>888</v>
       </c>
       <c r="G19" t="s">
@@ -13290,8 +13495,17 @@
       <c r="X19" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF19" t="s">
+        <v>926</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>927</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -13301,7 +13515,7 @@
       <c r="C20" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="26" t="s">
         <v>889</v>
       </c>
       <c r="G20" t="s">
@@ -13331,8 +13545,17 @@
       <c r="X20" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF20" t="s">
+        <v>929</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>930</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -13342,7 +13565,7 @@
       <c r="C21" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="56" t="s">
+      <c r="E21" s="26" t="s">
         <v>890</v>
       </c>
       <c r="G21" t="s">
@@ -13372,8 +13595,17 @@
       <c r="X21" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF21" t="s">
+        <v>932</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>933</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -13383,7 +13615,7 @@
       <c r="C22" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="56" t="s">
+      <c r="E22" s="26" t="s">
         <v>891</v>
       </c>
       <c r="G22" t="s">
@@ -13413,8 +13645,17 @@
       <c r="X22" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF22" t="s">
+        <v>935</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>936</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -13424,7 +13665,7 @@
       <c r="C23" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="26" t="s">
         <v>892</v>
       </c>
       <c r="G23" t="s">
@@ -13454,8 +13695,17 @@
       <c r="X23" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF23" t="s">
+        <v>938</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>939</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -13465,7 +13715,7 @@
       <c r="C24" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="26" t="s">
         <v>893</v>
       </c>
       <c r="G24" t="s">
@@ -13495,8 +13745,17 @@
       <c r="X24" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="AF24" t="s">
+        <v>941</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>942</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -13506,7 +13765,7 @@
       <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="26" t="s">
         <v>894</v>
       </c>
       <c r="G25" t="s">
@@ -13535,6 +13794,15 @@
       </c>
       <c r="X25" t="s">
         <v>507</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>944</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>945</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -13545,1113 +13813,1113 @@
     <mergeCell ref="E5:P5"/>
   </mergeCells>
   <conditionalFormatting sqref="A10:A9999">
-    <cfRule type="expression" dxfId="305" priority="1">
+    <cfRule type="expression" dxfId="302" priority="1">
       <formula>IF(VLOOKUP($A$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="304" priority="2">
+    <cfRule type="expression" dxfId="301" priority="2">
       <formula>IF(VLOOKUP($A$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="303" priority="3">
+    <cfRule type="expression" dxfId="300" priority="3">
       <formula>IF(VLOOKUP($A$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B9999">
-    <cfRule type="expression" dxfId="302" priority="4">
+    <cfRule type="expression" dxfId="299" priority="4">
       <formula>IF(VLOOKUP($B$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="301" priority="5">
+    <cfRule type="expression" dxfId="298" priority="5">
       <formula>IF(VLOOKUP($B$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="6">
+    <cfRule type="expression" dxfId="297" priority="6">
       <formula>IF(VLOOKUP($B$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C9999">
-    <cfRule type="expression" dxfId="299" priority="7">
+    <cfRule type="expression" dxfId="296" priority="7">
       <formula>IF(VLOOKUP($C$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="298" priority="8">
+    <cfRule type="expression" dxfId="295" priority="8">
       <formula>IF(VLOOKUP($C$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="297" priority="9">
+    <cfRule type="expression" dxfId="294" priority="9">
       <formula>IF(VLOOKUP($C$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D9999">
-    <cfRule type="expression" dxfId="296" priority="10">
+    <cfRule type="expression" dxfId="293" priority="10">
       <formula>IF(VLOOKUP($D$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="295" priority="11">
+    <cfRule type="expression" dxfId="292" priority="11">
       <formula>IF(VLOOKUP($D$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="294" priority="12">
+    <cfRule type="expression" dxfId="291" priority="12">
       <formula>IF(VLOOKUP($D$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E9999">
-    <cfRule type="expression" dxfId="293" priority="13">
+    <cfRule type="expression" dxfId="290" priority="13">
       <formula>IF(VLOOKUP($E$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="292" priority="14">
+    <cfRule type="expression" dxfId="289" priority="14">
       <formula>IF(VLOOKUP($E$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="291" priority="15">
+    <cfRule type="expression" dxfId="288" priority="15">
       <formula>IF(VLOOKUP($E$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:F9999">
-    <cfRule type="expression" dxfId="290" priority="16">
+    <cfRule type="expression" dxfId="287" priority="16">
       <formula>IF(VLOOKUP($F$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="289" priority="17">
+    <cfRule type="expression" dxfId="286" priority="17">
       <formula>IF(VLOOKUP($F$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="18">
+    <cfRule type="expression" dxfId="285" priority="18">
       <formula>IF(VLOOKUP($F$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:G9999">
-    <cfRule type="expression" dxfId="287" priority="19">
+    <cfRule type="expression" dxfId="284" priority="19">
       <formula>IF(VLOOKUP($G$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="20">
+    <cfRule type="expression" dxfId="283" priority="20">
       <formula>IF(VLOOKUP($G$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="285" priority="21">
+    <cfRule type="expression" dxfId="282" priority="21">
       <formula>IF(VLOOKUP($G$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:H9999">
-    <cfRule type="expression" dxfId="284" priority="22">
+    <cfRule type="expression" dxfId="281" priority="22">
       <formula>IF(VLOOKUP($H$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="23">
+    <cfRule type="expression" dxfId="280" priority="23">
       <formula>IF(VLOOKUP($H$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="24">
+    <cfRule type="expression" dxfId="279" priority="24">
       <formula>IF(VLOOKUP($H$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:I9999">
-    <cfRule type="expression" dxfId="281" priority="25">
+    <cfRule type="expression" dxfId="278" priority="25">
       <formula>IF(VLOOKUP($I$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="26">
+    <cfRule type="expression" dxfId="277" priority="26">
       <formula>IF(VLOOKUP($I$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="279" priority="27">
+    <cfRule type="expression" dxfId="276" priority="27">
       <formula>IF(VLOOKUP($I$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:J9999">
-    <cfRule type="expression" dxfId="278" priority="28">
+    <cfRule type="expression" dxfId="275" priority="28">
       <formula>IF(VLOOKUP($J$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="277" priority="29">
+    <cfRule type="expression" dxfId="274" priority="29">
       <formula>IF(VLOOKUP($J$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="276" priority="30">
+    <cfRule type="expression" dxfId="273" priority="30">
       <formula>IF(VLOOKUP($J$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:K9999">
-    <cfRule type="expression" dxfId="275" priority="31">
+    <cfRule type="expression" dxfId="272" priority="31">
       <formula>IF(VLOOKUP($K$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="274" priority="32">
+    <cfRule type="expression" dxfId="271" priority="32">
       <formula>IF(VLOOKUP($K$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="273" priority="33">
+    <cfRule type="expression" dxfId="270" priority="33">
       <formula>IF(VLOOKUP($K$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L9999">
-    <cfRule type="expression" dxfId="272" priority="34">
+    <cfRule type="expression" dxfId="269" priority="34">
       <formula>IF(VLOOKUP($L$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="271" priority="35">
+    <cfRule type="expression" dxfId="268" priority="35">
       <formula>IF(VLOOKUP($L$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="36">
+    <cfRule type="expression" dxfId="267" priority="36">
       <formula>IF(VLOOKUP($L$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:M9999">
-    <cfRule type="expression" dxfId="269" priority="37">
+    <cfRule type="expression" dxfId="266" priority="37">
       <formula>IF(VLOOKUP($M$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="38">
+    <cfRule type="expression" dxfId="265" priority="38">
       <formula>IF(VLOOKUP($M$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="39">
+    <cfRule type="expression" dxfId="264" priority="39">
       <formula>IF(VLOOKUP($M$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10:N9999">
-    <cfRule type="expression" dxfId="266" priority="40">
+    <cfRule type="expression" dxfId="263" priority="40">
       <formula>IF(VLOOKUP($N$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="265" priority="41">
+    <cfRule type="expression" dxfId="262" priority="41">
       <formula>IF(VLOOKUP($N$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="42">
+    <cfRule type="expression" dxfId="261" priority="42">
       <formula>IF(VLOOKUP($N$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O10:O9999">
-    <cfRule type="expression" dxfId="263" priority="43">
+    <cfRule type="expression" dxfId="260" priority="43">
       <formula>IF(VLOOKUP($O$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="44">
+    <cfRule type="expression" dxfId="259" priority="44">
       <formula>IF(VLOOKUP($O$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="261" priority="45">
+    <cfRule type="expression" dxfId="258" priority="45">
       <formula>IF(VLOOKUP($O$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10:P9999">
-    <cfRule type="expression" dxfId="26" priority="46">
+    <cfRule type="expression" dxfId="257" priority="46">
       <formula>IF(VLOOKUP($P$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="47">
+    <cfRule type="expression" dxfId="256" priority="47">
       <formula>IF(VLOOKUP($P$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="48">
+    <cfRule type="expression" dxfId="255" priority="48">
       <formula>IF(VLOOKUP($P$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:Q9999">
-    <cfRule type="expression" dxfId="23" priority="49">
+    <cfRule type="expression" dxfId="254" priority="49">
       <formula>IF(VLOOKUP($Q$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="50">
+    <cfRule type="expression" dxfId="253" priority="50">
       <formula>IF(VLOOKUP($Q$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="51">
+    <cfRule type="expression" dxfId="252" priority="51">
       <formula>IF(VLOOKUP($Q$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10:R9999">
-    <cfRule type="expression" dxfId="20" priority="52">
+    <cfRule type="expression" dxfId="251" priority="52">
       <formula>IF(VLOOKUP($R$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="53">
+    <cfRule type="expression" dxfId="250" priority="53">
       <formula>IF(VLOOKUP($R$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="54">
+    <cfRule type="expression" dxfId="249" priority="54">
       <formula>IF(VLOOKUP($R$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S9999">
-    <cfRule type="expression" dxfId="17" priority="55">
+    <cfRule type="expression" dxfId="248" priority="55">
       <formula>IF(VLOOKUP($S$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="56">
+    <cfRule type="expression" dxfId="247" priority="56">
       <formula>IF(VLOOKUP($S$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="57">
+    <cfRule type="expression" dxfId="246" priority="57">
       <formula>IF(VLOOKUP($S$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T10:T9999">
-    <cfRule type="expression" dxfId="14" priority="58">
+    <cfRule type="expression" dxfId="245" priority="58">
       <formula>IF(VLOOKUP($T$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="59">
+    <cfRule type="expression" dxfId="244" priority="59">
       <formula>IF(VLOOKUP($T$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="60">
+    <cfRule type="expression" dxfId="243" priority="60">
       <formula>IF(VLOOKUP($T$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U10:U9999">
-    <cfRule type="expression" dxfId="11" priority="61">
+    <cfRule type="expression" dxfId="242" priority="61">
       <formula>IF(VLOOKUP($U$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="62">
+    <cfRule type="expression" dxfId="241" priority="62">
       <formula>IF(VLOOKUP($U$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="63">
+    <cfRule type="expression" dxfId="240" priority="63">
       <formula>IF(VLOOKUP($U$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10:V9999">
-    <cfRule type="expression" dxfId="8" priority="64">
+    <cfRule type="expression" dxfId="239" priority="64">
       <formula>IF(VLOOKUP($V$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="65">
+    <cfRule type="expression" dxfId="238" priority="65">
       <formula>IF(VLOOKUP($V$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="66">
+    <cfRule type="expression" dxfId="237" priority="66">
       <formula>IF(VLOOKUP($V$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10:W9999">
-    <cfRule type="expression" dxfId="5" priority="67">
+    <cfRule type="expression" dxfId="236" priority="67">
       <formula>IF(VLOOKUP($W$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="68">
+    <cfRule type="expression" dxfId="235" priority="68">
       <formula>IF(VLOOKUP($W$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="69">
+    <cfRule type="expression" dxfId="234" priority="69">
       <formula>IF(VLOOKUP($W$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X10:X9999">
-    <cfRule type="expression" dxfId="2" priority="70">
+    <cfRule type="expression" dxfId="233" priority="70">
       <formula>IF(VLOOKUP($X$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="71">
+    <cfRule type="expression" dxfId="232" priority="71">
       <formula>IF(VLOOKUP($X$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="72">
+    <cfRule type="expression" dxfId="231" priority="72">
       <formula>IF(VLOOKUP($X$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y10:Y9999">
-    <cfRule type="expression" dxfId="260" priority="73">
+    <cfRule type="expression" dxfId="230" priority="73">
       <formula>IF(VLOOKUP($Y$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="259" priority="74">
+    <cfRule type="expression" dxfId="229" priority="74">
       <formula>IF(VLOOKUP($Y$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="75">
+    <cfRule type="expression" dxfId="228" priority="75">
       <formula>IF(VLOOKUP($Y$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z10:Z9999">
-    <cfRule type="expression" dxfId="257" priority="76">
+    <cfRule type="expression" dxfId="227" priority="76">
       <formula>IF(VLOOKUP($Z$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="77">
+    <cfRule type="expression" dxfId="226" priority="77">
       <formula>IF(VLOOKUP($Z$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="78">
+    <cfRule type="expression" dxfId="225" priority="78">
       <formula>IF(VLOOKUP($Z$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10:AA9999">
-    <cfRule type="expression" dxfId="254" priority="79">
+    <cfRule type="expression" dxfId="224" priority="79">
       <formula>IF(VLOOKUP($AA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="80">
+    <cfRule type="expression" dxfId="223" priority="80">
       <formula>IF(VLOOKUP($AA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="81">
+    <cfRule type="expression" dxfId="222" priority="81">
       <formula>IF(VLOOKUP($AA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10:AB9999">
-    <cfRule type="expression" dxfId="251" priority="82">
+    <cfRule type="expression" dxfId="221" priority="82">
       <formula>IF(VLOOKUP($AB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="83">
+    <cfRule type="expression" dxfId="220" priority="83">
       <formula>IF(VLOOKUP($AB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="249" priority="84">
+    <cfRule type="expression" dxfId="219" priority="84">
       <formula>IF(VLOOKUP($AB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC10:AC9999">
-    <cfRule type="expression" dxfId="248" priority="85">
+    <cfRule type="expression" dxfId="218" priority="85">
       <formula>IF(VLOOKUP($AC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="247" priority="86">
+    <cfRule type="expression" dxfId="217" priority="86">
       <formula>IF(VLOOKUP($AC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="87">
+    <cfRule type="expression" dxfId="216" priority="87">
       <formula>IF(VLOOKUP($AC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD10:AD9999">
-    <cfRule type="expression" dxfId="245" priority="88">
+    <cfRule type="expression" dxfId="215" priority="88">
       <formula>IF(VLOOKUP($AD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="89">
+    <cfRule type="expression" dxfId="214" priority="89">
       <formula>IF(VLOOKUP($AD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="90">
+    <cfRule type="expression" dxfId="213" priority="90">
       <formula>IF(VLOOKUP($AD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE10:AE9999">
-    <cfRule type="expression" dxfId="242" priority="91">
+    <cfRule type="expression" dxfId="212" priority="91">
       <formula>IF(VLOOKUP($AE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="92">
+    <cfRule type="expression" dxfId="211" priority="92">
       <formula>IF(VLOOKUP($AE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="93">
+    <cfRule type="expression" dxfId="210" priority="93">
       <formula>IF(VLOOKUP($AE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF10:AF9999">
-    <cfRule type="expression" dxfId="239" priority="94">
+    <cfRule type="expression" dxfId="209" priority="94">
       <formula>IF(VLOOKUP($AF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="95">
+    <cfRule type="expression" dxfId="208" priority="95">
       <formula>IF(VLOOKUP($AF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="96">
+    <cfRule type="expression" dxfId="207" priority="96">
       <formula>IF(VLOOKUP($AF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG10:AG9999">
-    <cfRule type="expression" dxfId="236" priority="97">
+    <cfRule type="expression" dxfId="206" priority="97">
       <formula>IF(VLOOKUP($AG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="98">
+    <cfRule type="expression" dxfId="205" priority="98">
       <formula>IF(VLOOKUP($AG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="99">
+    <cfRule type="expression" dxfId="204" priority="99">
       <formula>IF(VLOOKUP($AG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH10:AH9999">
-    <cfRule type="expression" dxfId="233" priority="100">
+    <cfRule type="expression" dxfId="203" priority="100">
       <formula>IF(VLOOKUP($AH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="101">
+    <cfRule type="expression" dxfId="202" priority="101">
       <formula>IF(VLOOKUP($AH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="102">
+    <cfRule type="expression" dxfId="201" priority="102">
       <formula>IF(VLOOKUP($AH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI10:AI9999">
-    <cfRule type="expression" dxfId="230" priority="103">
+    <cfRule type="expression" dxfId="200" priority="103">
       <formula>IF(VLOOKUP($AI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="104">
+    <cfRule type="expression" dxfId="199" priority="104">
       <formula>IF(VLOOKUP($AI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="105">
+    <cfRule type="expression" dxfId="198" priority="105">
       <formula>IF(VLOOKUP($AI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10:AJ9999">
-    <cfRule type="expression" dxfId="227" priority="106">
+    <cfRule type="expression" dxfId="197" priority="106">
       <formula>IF(VLOOKUP($AJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="107">
+    <cfRule type="expression" dxfId="196" priority="107">
       <formula>IF(VLOOKUP($AJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="108">
+    <cfRule type="expression" dxfId="195" priority="108">
       <formula>IF(VLOOKUP($AJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK10:AK9999">
-    <cfRule type="expression" dxfId="224" priority="109">
+    <cfRule type="expression" dxfId="194" priority="109">
       <formula>IF(VLOOKUP($AK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="110">
+    <cfRule type="expression" dxfId="193" priority="110">
       <formula>IF(VLOOKUP($AK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="111">
+    <cfRule type="expression" dxfId="192" priority="111">
       <formula>IF(VLOOKUP($AK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL10:AL9999">
-    <cfRule type="expression" dxfId="221" priority="112">
+    <cfRule type="expression" dxfId="191" priority="112">
       <formula>IF(VLOOKUP($AL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="113">
+    <cfRule type="expression" dxfId="190" priority="113">
       <formula>IF(VLOOKUP($AL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="114">
+    <cfRule type="expression" dxfId="189" priority="114">
       <formula>IF(VLOOKUP($AL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM10:AM9999">
-    <cfRule type="expression" dxfId="218" priority="115">
+    <cfRule type="expression" dxfId="188" priority="115">
       <formula>IF(VLOOKUP($AM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="116">
+    <cfRule type="expression" dxfId="187" priority="116">
       <formula>IF(VLOOKUP($AM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="117">
+    <cfRule type="expression" dxfId="186" priority="117">
       <formula>IF(VLOOKUP($AM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN10:AN9999">
-    <cfRule type="expression" dxfId="215" priority="118">
+    <cfRule type="expression" dxfId="185" priority="118">
       <formula>IF(VLOOKUP($AN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="119">
+    <cfRule type="expression" dxfId="184" priority="119">
       <formula>IF(VLOOKUP($AN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="120">
+    <cfRule type="expression" dxfId="183" priority="120">
       <formula>IF(VLOOKUP($AN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO10:AO9999">
-    <cfRule type="expression" dxfId="212" priority="121">
+    <cfRule type="expression" dxfId="182" priority="121">
       <formula>IF(VLOOKUP($AO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="122">
+    <cfRule type="expression" dxfId="181" priority="122">
       <formula>IF(VLOOKUP($AO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="123">
+    <cfRule type="expression" dxfId="180" priority="123">
       <formula>IF(VLOOKUP($AO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP10:AP9999">
-    <cfRule type="expression" dxfId="209" priority="124">
+    <cfRule type="expression" dxfId="179" priority="124">
       <formula>IF(VLOOKUP($AP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="125">
+    <cfRule type="expression" dxfId="178" priority="125">
       <formula>IF(VLOOKUP($AP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="207" priority="126">
+    <cfRule type="expression" dxfId="177" priority="126">
       <formula>IF(VLOOKUP($AP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ10:AQ9999">
-    <cfRule type="expression" dxfId="206" priority="127">
+    <cfRule type="expression" dxfId="176" priority="127">
       <formula>IF(VLOOKUP($AQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="128">
+    <cfRule type="expression" dxfId="175" priority="128">
       <formula>IF(VLOOKUP($AQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="129">
+    <cfRule type="expression" dxfId="174" priority="129">
       <formula>IF(VLOOKUP($AQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR10:AR9999">
-    <cfRule type="expression" dxfId="203" priority="130">
+    <cfRule type="expression" dxfId="173" priority="130">
       <formula>IF(VLOOKUP($AR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="131">
+    <cfRule type="expression" dxfId="172" priority="131">
       <formula>IF(VLOOKUP($AR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="132">
+    <cfRule type="expression" dxfId="171" priority="132">
       <formula>IF(VLOOKUP($AR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS10:AS9999">
-    <cfRule type="expression" dxfId="200" priority="133">
+    <cfRule type="expression" dxfId="170" priority="133">
       <formula>IF(VLOOKUP($AS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="134">
+    <cfRule type="expression" dxfId="169" priority="134">
       <formula>IF(VLOOKUP($AS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="135">
+    <cfRule type="expression" dxfId="168" priority="135">
       <formula>IF(VLOOKUP($AS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT10:AT9999">
-    <cfRule type="expression" dxfId="197" priority="136">
+    <cfRule type="expression" dxfId="167" priority="136">
       <formula>IF(VLOOKUP($AT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="137">
+    <cfRule type="expression" dxfId="166" priority="137">
       <formula>IF(VLOOKUP($AT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="138">
+    <cfRule type="expression" dxfId="165" priority="138">
       <formula>IF(VLOOKUP($AT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU10:AU9999">
-    <cfRule type="expression" dxfId="194" priority="139">
+    <cfRule type="expression" dxfId="164" priority="139">
       <formula>IF(VLOOKUP($AU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="140">
+    <cfRule type="expression" dxfId="163" priority="140">
       <formula>IF(VLOOKUP($AU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="141">
+    <cfRule type="expression" dxfId="162" priority="141">
       <formula>IF(VLOOKUP($AU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV10:AV9999">
-    <cfRule type="expression" dxfId="191" priority="142">
+    <cfRule type="expression" dxfId="161" priority="142">
       <formula>IF(VLOOKUP($AV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="143">
+    <cfRule type="expression" dxfId="160" priority="143">
       <formula>IF(VLOOKUP($AV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="144">
+    <cfRule type="expression" dxfId="159" priority="144">
       <formula>IF(VLOOKUP($AV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW10:AW9999">
-    <cfRule type="expression" dxfId="188" priority="145">
+    <cfRule type="expression" dxfId="158" priority="145">
       <formula>IF(VLOOKUP($AW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="146">
+    <cfRule type="expression" dxfId="157" priority="146">
       <formula>IF(VLOOKUP($AW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="147">
+    <cfRule type="expression" dxfId="156" priority="147">
       <formula>IF(VLOOKUP($AW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX10:AX9999">
-    <cfRule type="expression" dxfId="185" priority="148">
+    <cfRule type="expression" dxfId="155" priority="148">
       <formula>IF(VLOOKUP($AX$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="149">
+    <cfRule type="expression" dxfId="154" priority="149">
       <formula>IF(VLOOKUP($AX$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="150">
+    <cfRule type="expression" dxfId="153" priority="150">
       <formula>IF(VLOOKUP($AX$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY10:AY9999">
-    <cfRule type="expression" dxfId="182" priority="151">
+    <cfRule type="expression" dxfId="152" priority="151">
       <formula>IF(VLOOKUP($AY$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="152">
+    <cfRule type="expression" dxfId="151" priority="152">
       <formula>IF(VLOOKUP($AY$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="153">
+    <cfRule type="expression" dxfId="150" priority="153">
       <formula>IF(VLOOKUP($AY$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ10:AZ9999">
-    <cfRule type="expression" dxfId="179" priority="154">
+    <cfRule type="expression" dxfId="149" priority="154">
       <formula>IF(VLOOKUP($AZ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="155">
+    <cfRule type="expression" dxfId="148" priority="155">
       <formula>IF(VLOOKUP($AZ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="156">
+    <cfRule type="expression" dxfId="147" priority="156">
       <formula>IF(VLOOKUP($AZ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA10:BA9999">
-    <cfRule type="expression" dxfId="176" priority="157">
+    <cfRule type="expression" dxfId="146" priority="157">
       <formula>IF(VLOOKUP($BA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="158">
+    <cfRule type="expression" dxfId="145" priority="158">
       <formula>IF(VLOOKUP($BA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="159">
+    <cfRule type="expression" dxfId="144" priority="159">
       <formula>IF(VLOOKUP($BA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB10:BB9999">
-    <cfRule type="expression" dxfId="173" priority="160">
+    <cfRule type="expression" dxfId="143" priority="160">
       <formula>IF(VLOOKUP($BB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="161">
+    <cfRule type="expression" dxfId="142" priority="161">
       <formula>IF(VLOOKUP($BB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="162">
+    <cfRule type="expression" dxfId="141" priority="162">
       <formula>IF(VLOOKUP($BB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC10:BC9999">
-    <cfRule type="expression" dxfId="170" priority="163">
+    <cfRule type="expression" dxfId="140" priority="163">
       <formula>IF(VLOOKUP($BC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="164">
+    <cfRule type="expression" dxfId="139" priority="164">
       <formula>IF(VLOOKUP($BC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="165">
+    <cfRule type="expression" dxfId="138" priority="165">
       <formula>IF(VLOOKUP($BC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD10:BD9999">
-    <cfRule type="expression" dxfId="167" priority="166">
+    <cfRule type="expression" dxfId="137" priority="166">
       <formula>IF(VLOOKUP($BD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="167">
+    <cfRule type="expression" dxfId="136" priority="167">
       <formula>IF(VLOOKUP($BD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="168">
+    <cfRule type="expression" dxfId="135" priority="168">
       <formula>IF(VLOOKUP($BD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE10:BE9999">
-    <cfRule type="expression" dxfId="164" priority="169">
+    <cfRule type="expression" dxfId="134" priority="169">
       <formula>IF(VLOOKUP($BE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="170">
+    <cfRule type="expression" dxfId="133" priority="170">
       <formula>IF(VLOOKUP($BE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="171">
+    <cfRule type="expression" dxfId="132" priority="171">
       <formula>IF(VLOOKUP($BE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF10:BF9999">
-    <cfRule type="expression" dxfId="161" priority="172">
+    <cfRule type="expression" dxfId="131" priority="172">
       <formula>IF(VLOOKUP($BF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="173">
+    <cfRule type="expression" dxfId="130" priority="173">
       <formula>IF(VLOOKUP($BF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="174">
+    <cfRule type="expression" dxfId="129" priority="174">
       <formula>IF(VLOOKUP($BF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG10:BG9999">
-    <cfRule type="expression" dxfId="158" priority="175">
+    <cfRule type="expression" dxfId="128" priority="175">
       <formula>IF(VLOOKUP($BG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="176">
+    <cfRule type="expression" dxfId="127" priority="176">
       <formula>IF(VLOOKUP($BG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="177">
+    <cfRule type="expression" dxfId="126" priority="177">
       <formula>IF(VLOOKUP($BG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH10:BH9999">
-    <cfRule type="expression" dxfId="155" priority="178">
+    <cfRule type="expression" dxfId="125" priority="178">
       <formula>IF(VLOOKUP($BH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="179">
+    <cfRule type="expression" dxfId="124" priority="179">
       <formula>IF(VLOOKUP($BH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="180">
+    <cfRule type="expression" dxfId="123" priority="180">
       <formula>IF(VLOOKUP($BH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI10:BI9999">
-    <cfRule type="expression" dxfId="152" priority="181">
+    <cfRule type="expression" dxfId="122" priority="181">
       <formula>IF(VLOOKUP($BI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="182">
+    <cfRule type="expression" dxfId="121" priority="182">
       <formula>IF(VLOOKUP($BI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="183">
+    <cfRule type="expression" dxfId="120" priority="183">
       <formula>IF(VLOOKUP($BI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ10:BJ9999">
-    <cfRule type="expression" dxfId="149" priority="184">
+    <cfRule type="expression" dxfId="119" priority="184">
       <formula>IF(VLOOKUP($BJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="185">
+    <cfRule type="expression" dxfId="118" priority="185">
       <formula>IF(VLOOKUP($BJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="186">
+    <cfRule type="expression" dxfId="117" priority="186">
       <formula>IF(VLOOKUP($BJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK10:BK9999">
-    <cfRule type="expression" dxfId="146" priority="187">
+    <cfRule type="expression" dxfId="116" priority="187">
       <formula>IF(VLOOKUP($BK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="188">
+    <cfRule type="expression" dxfId="115" priority="188">
       <formula>IF(VLOOKUP($BK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="189">
+    <cfRule type="expression" dxfId="114" priority="189">
       <formula>IF(VLOOKUP($BK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL10:BL9999">
-    <cfRule type="expression" dxfId="143" priority="190">
+    <cfRule type="expression" dxfId="113" priority="190">
       <formula>IF(VLOOKUP($BL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="191">
+    <cfRule type="expression" dxfId="112" priority="191">
       <formula>IF(VLOOKUP($BL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="192">
+    <cfRule type="expression" dxfId="111" priority="192">
       <formula>IF(VLOOKUP($BL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM10:BM9999">
-    <cfRule type="expression" dxfId="140" priority="193">
+    <cfRule type="expression" dxfId="110" priority="193">
       <formula>IF(VLOOKUP($BM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="194">
+    <cfRule type="expression" dxfId="109" priority="194">
       <formula>IF(VLOOKUP($BM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="195">
+    <cfRule type="expression" dxfId="108" priority="195">
       <formula>IF(VLOOKUP($BM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN10:BN9999">
-    <cfRule type="expression" dxfId="137" priority="196">
+    <cfRule type="expression" dxfId="107" priority="196">
       <formula>IF(VLOOKUP($BN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="197">
+    <cfRule type="expression" dxfId="106" priority="197">
       <formula>IF(VLOOKUP($BN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="198">
+    <cfRule type="expression" dxfId="105" priority="198">
       <formula>IF(VLOOKUP($BN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO10:BO9999">
-    <cfRule type="expression" dxfId="134" priority="199">
+    <cfRule type="expression" dxfId="104" priority="199">
       <formula>IF(VLOOKUP($BO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="200">
+    <cfRule type="expression" dxfId="103" priority="200">
       <formula>IF(VLOOKUP($BO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="201">
+    <cfRule type="expression" dxfId="102" priority="201">
       <formula>IF(VLOOKUP($BO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP10:BP9999">
-    <cfRule type="expression" dxfId="131" priority="202">
+    <cfRule type="expression" dxfId="101" priority="202">
       <formula>IF(VLOOKUP($BP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="203">
+    <cfRule type="expression" dxfId="100" priority="203">
       <formula>IF(VLOOKUP($BP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="204">
+    <cfRule type="expression" dxfId="99" priority="204">
       <formula>IF(VLOOKUP($BP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ10:BQ9999">
-    <cfRule type="expression" dxfId="128" priority="205">
+    <cfRule type="expression" dxfId="98" priority="205">
       <formula>IF(VLOOKUP($BQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="206">
+    <cfRule type="expression" dxfId="97" priority="206">
       <formula>IF(VLOOKUP($BQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="207">
+    <cfRule type="expression" dxfId="96" priority="207">
       <formula>IF(VLOOKUP($BQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR10:BR9999">
-    <cfRule type="expression" dxfId="125" priority="208">
+    <cfRule type="expression" dxfId="95" priority="208">
       <formula>IF(VLOOKUP($BR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="209">
+    <cfRule type="expression" dxfId="94" priority="209">
       <formula>IF(VLOOKUP($BR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="210">
+    <cfRule type="expression" dxfId="93" priority="210">
       <formula>IF(VLOOKUP($BR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS10:BS9999">
-    <cfRule type="expression" dxfId="122" priority="211">
+    <cfRule type="expression" dxfId="92" priority="211">
       <formula>IF(VLOOKUP($BS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="212">
+    <cfRule type="expression" dxfId="91" priority="212">
       <formula>IF(VLOOKUP($BS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="213">
+    <cfRule type="expression" dxfId="90" priority="213">
       <formula>IF(VLOOKUP($BS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT10:BT9999">
-    <cfRule type="expression" dxfId="119" priority="214">
+    <cfRule type="expression" dxfId="89" priority="214">
       <formula>IF(VLOOKUP($BT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="215">
+    <cfRule type="expression" dxfId="88" priority="215">
       <formula>IF(VLOOKUP($BT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="216">
+    <cfRule type="expression" dxfId="87" priority="216">
       <formula>IF(VLOOKUP($BT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU10:BU9999">
-    <cfRule type="expression" dxfId="116" priority="217">
+    <cfRule type="expression" dxfId="86" priority="217">
       <formula>IF(VLOOKUP($BU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="218">
+    <cfRule type="expression" dxfId="85" priority="218">
       <formula>IF(VLOOKUP($BU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="219">
+    <cfRule type="expression" dxfId="84" priority="219">
       <formula>IF(VLOOKUP($BU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV10:BV9999">
-    <cfRule type="expression" dxfId="113" priority="220">
+    <cfRule type="expression" dxfId="83" priority="220">
       <formula>IF(VLOOKUP($BV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="221">
+    <cfRule type="expression" dxfId="82" priority="221">
       <formula>IF(VLOOKUP($BV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="222">
+    <cfRule type="expression" dxfId="81" priority="222">
       <formula>IF(VLOOKUP($BV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BW10:BW9999">
-    <cfRule type="expression" dxfId="110" priority="223">
+    <cfRule type="expression" dxfId="80" priority="223">
       <formula>IF(VLOOKUP($BW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="224">
+    <cfRule type="expression" dxfId="79" priority="224">
       <formula>IF(VLOOKUP($BW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="225">
+    <cfRule type="expression" dxfId="78" priority="225">
       <formula>IF(VLOOKUP($BW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX10:BX9999">
-    <cfRule type="expression" dxfId="107" priority="226">
+    <cfRule type="expression" dxfId="77" priority="226">
       <formula>IF(VLOOKUP($BX$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="227">
+    <cfRule type="expression" dxfId="76" priority="227">
       <formula>IF(VLOOKUP($BX$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="228">
+    <cfRule type="expression" dxfId="75" priority="228">
       <formula>IF(VLOOKUP($BX$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BY10:BY9999">
-    <cfRule type="expression" dxfId="104" priority="229">
+    <cfRule type="expression" dxfId="74" priority="229">
       <formula>IF(VLOOKUP($BY$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="230">
+    <cfRule type="expression" dxfId="73" priority="230">
       <formula>IF(VLOOKUP($BY$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="231">
+    <cfRule type="expression" dxfId="72" priority="231">
       <formula>IF(VLOOKUP($BY$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BZ10:BZ9999">
-    <cfRule type="expression" dxfId="101" priority="232">
+    <cfRule type="expression" dxfId="71" priority="232">
       <formula>IF(VLOOKUP($BZ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="233">
+    <cfRule type="expression" dxfId="70" priority="233">
       <formula>IF(VLOOKUP($BZ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="234">
+    <cfRule type="expression" dxfId="69" priority="234">
       <formula>IF(VLOOKUP($BZ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA10:CA9999">
-    <cfRule type="expression" dxfId="98" priority="235">
+    <cfRule type="expression" dxfId="68" priority="235">
       <formula>IF(VLOOKUP($CA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="236">
+    <cfRule type="expression" dxfId="67" priority="236">
       <formula>IF(VLOOKUP($CA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="237">
+    <cfRule type="expression" dxfId="66" priority="237">
       <formula>IF(VLOOKUP($CA$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CB10:CB9999">
-    <cfRule type="expression" dxfId="95" priority="238">
+    <cfRule type="expression" dxfId="65" priority="238">
       <formula>IF(VLOOKUP($CB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="239">
+    <cfRule type="expression" dxfId="64" priority="239">
       <formula>IF(VLOOKUP($CB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="240">
+    <cfRule type="expression" dxfId="63" priority="240">
       <formula>IF(VLOOKUP($CB$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CC10:CC9999">
-    <cfRule type="expression" dxfId="92" priority="241">
+    <cfRule type="expression" dxfId="62" priority="241">
       <formula>IF(VLOOKUP($CC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="242">
+    <cfRule type="expression" dxfId="61" priority="242">
       <formula>IF(VLOOKUP($CC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="243">
+    <cfRule type="expression" dxfId="60" priority="243">
       <formula>IF(VLOOKUP($CC$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CD10:CD9999">
-    <cfRule type="expression" dxfId="89" priority="244">
+    <cfRule type="expression" dxfId="59" priority="244">
       <formula>IF(VLOOKUP($CD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="245">
+    <cfRule type="expression" dxfId="58" priority="245">
       <formula>IF(VLOOKUP($CD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="246">
+    <cfRule type="expression" dxfId="57" priority="246">
       <formula>IF(VLOOKUP($CD$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CE10:CE9999">
-    <cfRule type="expression" dxfId="86" priority="247">
+    <cfRule type="expression" dxfId="56" priority="247">
       <formula>IF(VLOOKUP($CE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="248">
+    <cfRule type="expression" dxfId="55" priority="248">
       <formula>IF(VLOOKUP($CE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="249">
+    <cfRule type="expression" dxfId="54" priority="249">
       <formula>IF(VLOOKUP($CE$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CF10:CF9999">
-    <cfRule type="expression" dxfId="83" priority="250">
+    <cfRule type="expression" dxfId="53" priority="250">
       <formula>IF(VLOOKUP($CF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="251">
+    <cfRule type="expression" dxfId="52" priority="251">
       <formula>IF(VLOOKUP($CF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="252">
+    <cfRule type="expression" dxfId="51" priority="252">
       <formula>IF(VLOOKUP($CF$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CG10:CG9999">
-    <cfRule type="expression" dxfId="80" priority="253">
+    <cfRule type="expression" dxfId="50" priority="253">
       <formula>IF(VLOOKUP($CG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="254">
+    <cfRule type="expression" dxfId="49" priority="254">
       <formula>IF(VLOOKUP($CG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="255">
+    <cfRule type="expression" dxfId="48" priority="255">
       <formula>IF(VLOOKUP($CG$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CH10:CH9999">
-    <cfRule type="expression" dxfId="77" priority="256">
+    <cfRule type="expression" dxfId="47" priority="256">
       <formula>IF(VLOOKUP($CH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="257">
+    <cfRule type="expression" dxfId="46" priority="257">
       <formula>IF(VLOOKUP($CH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="258">
+    <cfRule type="expression" dxfId="45" priority="258">
       <formula>IF(VLOOKUP($CH$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CI10:CI9999">
-    <cfRule type="expression" dxfId="74" priority="259">
+    <cfRule type="expression" dxfId="44" priority="259">
       <formula>IF(VLOOKUP($CI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="260">
+    <cfRule type="expression" dxfId="43" priority="260">
       <formula>IF(VLOOKUP($CI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="261">
+    <cfRule type="expression" dxfId="42" priority="261">
       <formula>IF(VLOOKUP($CI$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ10:CJ9999">
-    <cfRule type="expression" dxfId="71" priority="262">
+    <cfRule type="expression" dxfId="41" priority="262">
       <formula>IF(VLOOKUP($CJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="263">
+    <cfRule type="expression" dxfId="40" priority="263">
       <formula>IF(VLOOKUP($CJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="264">
+    <cfRule type="expression" dxfId="39" priority="264">
       <formula>IF(VLOOKUP($CJ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CK10:CK9999">
-    <cfRule type="expression" dxfId="68" priority="265">
+    <cfRule type="expression" dxfId="38" priority="265">
       <formula>IF(VLOOKUP($CK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="266">
+    <cfRule type="expression" dxfId="37" priority="266">
       <formula>IF(VLOOKUP($CK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="267">
+    <cfRule type="expression" dxfId="36" priority="267">
       <formula>IF(VLOOKUP($CK$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL10:CL9999">
-    <cfRule type="expression" dxfId="65" priority="268">
+    <cfRule type="expression" dxfId="35" priority="268">
       <formula>IF(VLOOKUP($CL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="269">
+    <cfRule type="expression" dxfId="34" priority="269">
       <formula>IF(VLOOKUP($CL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="270">
+    <cfRule type="expression" dxfId="33" priority="270">
       <formula>IF(VLOOKUP($CL$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CM10:CM9999">
-    <cfRule type="expression" dxfId="62" priority="271">
+    <cfRule type="expression" dxfId="32" priority="271">
       <formula>IF(VLOOKUP($CM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="272">
+    <cfRule type="expression" dxfId="31" priority="272">
       <formula>IF(VLOOKUP($CM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="273">
+    <cfRule type="expression" dxfId="30" priority="273">
       <formula>IF(VLOOKUP($CM$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CN10:CN9999">
-    <cfRule type="expression" dxfId="59" priority="274">
+    <cfRule type="expression" dxfId="29" priority="274">
       <formula>IF(VLOOKUP($CN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="275">
+    <cfRule type="expression" dxfId="28" priority="275">
       <formula>IF(VLOOKUP($CN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="276">
+    <cfRule type="expression" dxfId="27" priority="276">
       <formula>IF(VLOOKUP($CN$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO10:CO9999">
-    <cfRule type="expression" dxfId="56" priority="277">
+    <cfRule type="expression" dxfId="26" priority="277">
       <formula>IF(VLOOKUP($CO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="278">
+    <cfRule type="expression" dxfId="25" priority="278">
       <formula>IF(VLOOKUP($CO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="279">
+    <cfRule type="expression" dxfId="24" priority="279">
       <formula>IF(VLOOKUP($CO$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP10:CP9999">
-    <cfRule type="expression" dxfId="53" priority="280">
+    <cfRule type="expression" dxfId="23" priority="280">
       <formula>IF(VLOOKUP($CP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="281">
+    <cfRule type="expression" dxfId="22" priority="281">
       <formula>IF(VLOOKUP($CP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="282">
+    <cfRule type="expression" dxfId="21" priority="282">
       <formula>IF(VLOOKUP($CP$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CQ10:CQ9999">
-    <cfRule type="expression" dxfId="50" priority="283">
+    <cfRule type="expression" dxfId="20" priority="283">
       <formula>IF(VLOOKUP($CQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="284">
+    <cfRule type="expression" dxfId="19" priority="284">
       <formula>IF(VLOOKUP($CQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="285">
+    <cfRule type="expression" dxfId="18" priority="285">
       <formula>IF(VLOOKUP($CQ$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CR10:CR9999">
-    <cfRule type="expression" dxfId="47" priority="286">
+    <cfRule type="expression" dxfId="17" priority="286">
       <formula>IF(VLOOKUP($CR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="287">
+    <cfRule type="expression" dxfId="16" priority="287">
       <formula>IF(VLOOKUP($CR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="288">
+    <cfRule type="expression" dxfId="15" priority="288">
       <formula>IF(VLOOKUP($CR$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CS10:CS9999">
-    <cfRule type="expression" dxfId="44" priority="289">
+    <cfRule type="expression" dxfId="14" priority="289">
       <formula>IF(VLOOKUP($CS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="290">
+    <cfRule type="expression" dxfId="13" priority="290">
       <formula>IF(VLOOKUP($CS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="291">
+    <cfRule type="expression" dxfId="12" priority="291">
       <formula>IF(VLOOKUP($CS$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CT10:CT9999">
-    <cfRule type="expression" dxfId="41" priority="292">
+    <cfRule type="expression" dxfId="11" priority="292">
       <formula>IF(VLOOKUP($CT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="293">
+    <cfRule type="expression" dxfId="10" priority="293">
       <formula>IF(VLOOKUP($CT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="294">
+    <cfRule type="expression" dxfId="9" priority="294">
       <formula>IF(VLOOKUP($CT$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CU10:CU9999">
-    <cfRule type="expression" dxfId="38" priority="295">
+    <cfRule type="expression" dxfId="8" priority="295">
       <formula>IF(VLOOKUP($CU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="296">
+    <cfRule type="expression" dxfId="7" priority="296">
       <formula>IF(VLOOKUP($CU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="297">
+    <cfRule type="expression" dxfId="6" priority="297">
       <formula>IF(VLOOKUP($CU$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CV10:CV9999">
-    <cfRule type="expression" dxfId="35" priority="298">
+    <cfRule type="expression" dxfId="5" priority="298">
       <formula>IF(VLOOKUP($CV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="299">
+    <cfRule type="expression" dxfId="4" priority="299">
       <formula>IF(VLOOKUP($CV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="300">
+    <cfRule type="expression" dxfId="3" priority="300">
       <formula>IF(VLOOKUP($CV$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CW10:CW9999">
-    <cfRule type="expression" dxfId="32" priority="301">
+    <cfRule type="expression" dxfId="2" priority="301">
       <formula>IF(VLOOKUP($CW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=2,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="302">
+    <cfRule type="expression" dxfId="1" priority="302">
       <formula>IF(VLOOKUP($CW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=1,1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="303">
+    <cfRule type="expression" dxfId="0" priority="303">
       <formula>IF(VLOOKUP($CW$9,requiredAttributePTDMap,MATCH(LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($C10," ", "_"),"&amp;",""),",",""),"--","-"),"-","_"),"/","_"),"__","_")),attributeMapFeedProductType,0)+1,FALSE)=-1,1,0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14781,8 +15049,11 @@
       <formula1>valid_values_vat_rate_eg</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AG16" r:id="rId1" xr:uid="{32367BCE-6447-480B-A044-0EDF4F1C7B73}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>